<commit_message>
Adding more data to Kd comparison table
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -13,7 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Compilation" sheetId="1" r:id="rId1"/>
-    <sheet name="Sajih Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Ames Data" sheetId="4" r:id="rId2"/>
+    <sheet name="Sajih Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Nirdosh Data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="63">
   <si>
     <t>Sorption Isotherm Comparison</t>
   </si>
@@ -175,6 +177,45 @@
   </si>
   <si>
     <t>Lepidocrocite</t>
+  </si>
+  <si>
+    <t>pH 1 solution</t>
+  </si>
+  <si>
+    <t>pH 10 solution</t>
+  </si>
+  <si>
+    <t>Nirdosh, Reported</t>
+  </si>
+  <si>
+    <t>Solid Ra (Bq/g)</t>
+  </si>
+  <si>
+    <t>Tot Ra (Bq/mL)</t>
+  </si>
+  <si>
+    <t>Free Ra (Bq/mL filtrate)</t>
+  </si>
+  <si>
+    <t>pH 1</t>
+  </si>
+  <si>
+    <t>Nirdosh, from digitized data</t>
+  </si>
+  <si>
+    <t>Free Ra (mol/L)</t>
+  </si>
+  <si>
+    <t>Solid Ra (mol/g)</t>
+  </si>
+  <si>
+    <t>Free Ra (mol/mL)</t>
+  </si>
+  <si>
+    <t>Ames, 1983</t>
+  </si>
+  <si>
+    <t>Sodium Montmorillonite</t>
   </si>
 </sst>
 </file>
@@ -238,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -248,6 +289,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,6 +306,918 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nirdosh</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Nirdosh Data'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Nirdosh Data'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5840000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0139999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.455999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="256494544"/>
+        <c:axId val="256493760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="256494544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="256493760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="256493760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="256494544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,12 +1817,362 @@
         <v>43</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0.752</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <v>10.1</v>
+      </c>
+      <c r="E18">
+        <v>544</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <f>1/20</f>
+        <v>0.05</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>6.5</v>
+      </c>
+      <c r="E19">
+        <v>3724</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1.395E-9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5.1799999999999999E-9</v>
+      </c>
+      <c r="C2" s="5">
+        <f>A2/1000</f>
+        <v>1.395E-12</v>
+      </c>
+      <c r="D2" s="6">
+        <f>B2/C2</f>
+        <v>3713.2616487455198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1.469E-10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5.2800000000000004E-10</v>
+      </c>
+      <c r="C3" s="5">
+        <f>A3/1000</f>
+        <v>1.4690000000000001E-13</v>
+      </c>
+      <c r="D3" s="6">
+        <f>B3/C3</f>
+        <v>3594.28182437032</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1.822E-11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>5.5600000000000001E-11</v>
+      </c>
+      <c r="C4" s="5">
+        <f>A4/1000</f>
+        <v>1.822E-14</v>
+      </c>
+      <c r="D4" s="6">
+        <f>B4/C4</f>
+        <v>3051.5916575192095</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.99999926963558483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.99999853927170312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="6"/>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.99999707854340625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4.8406511408979136E-12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.6041223608096529E-17</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.6041223608096529E-17</v>
+      </c>
+      <c r="J12" s="1">
+        <v>684589.0104526967</v>
+      </c>
+      <c r="K12" s="1">
+        <v>7.6942262009724945E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2.3431903467876272E-23</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.3431903467876272E-23</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.6041247039999997E-17</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-1.549705240455168E-11</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3.6454815285820572E-12</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-4.2510302913479299</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.14708248777795169</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-6.1817287068658424E-11</v>
+      </c>
+      <c r="L17" s="1">
+        <v>3.0823182259555064E-11</v>
+      </c>
+      <c r="M17" s="1">
+        <v>-6.1817287068658424E-11</v>
+      </c>
+      <c r="N17" s="1">
+        <v>3.0823182259555064E-11</v>
+      </c>
+    </row>
+    <row r="18" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3724.1309368597631</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4.5010100260851598</v>
+      </c>
+      <c r="I18" s="2">
+        <v>827.39894274327969</v>
+      </c>
+      <c r="J18" s="2">
+        <v>7.6942262009724934E-4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3666.9401819487498</v>
+      </c>
+      <c r="L18" s="2">
+        <v>3781.3216917707764</v>
+      </c>
+      <c r="M18" s="2">
+        <v>3666.9401819487498</v>
+      </c>
+      <c r="N18" s="2">
+        <v>3781.3216917707764</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
@@ -1401,4 +2706,479 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.2</v>
+      </c>
+      <c r="B2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <f>(A2-B2)*10/5</f>
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="D2">
+        <v>11.4</v>
+      </c>
+      <c r="E2">
+        <f>C2/B2</f>
+        <v>64.666666666666671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.4</v>
+      </c>
+      <c r="B3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C8" si="0">(A3-B3)*10/5</f>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="D3">
+        <v>10.8</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="1">C3/B3</f>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.8</v>
+      </c>
+      <c r="B4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.5840000000000001</v>
+      </c>
+      <c r="D4">
+        <v>9.4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.73</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.44</v>
+      </c>
+      <c r="D5">
+        <v>10.1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.64</v>
+      </c>
+      <c r="B6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>7.2640000000000002</v>
+      </c>
+      <c r="D6">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>908</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.55</v>
+      </c>
+      <c r="B7">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>9.0139999999999993</v>
+      </c>
+      <c r="D7">
+        <v>9.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>209.62790697674419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>22.74</v>
+      </c>
+      <c r="B8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>45.455999999999996</v>
+      </c>
+      <c r="D8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>3787.9999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.33537894000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.17190375999999999</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>C9/B9</f>
+        <v>0.51256575621593881</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.64073210000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.51164936999999999</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E14" si="2">C10/B10</f>
+        <v>0.79853868722981103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1.2517366000000001</v>
+      </c>
+      <c r="C11">
+        <v>1.0652086000000001</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0.85098462408145614</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1.6840321</v>
+      </c>
+      <c r="C12">
+        <v>2.0155327000000001</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>1.1968493355916434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>7.5865210000000003</v>
+      </c>
+      <c r="C13">
+        <v>7.6184609999999999</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>1.0042100984100617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>16.631900000000002</v>
+      </c>
+      <c r="C14">
+        <v>12.250152999999999</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>0.73654561415111908</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.98626833922986679</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.97272523696723956</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.96590654620904948</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.90648738595015843</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>117.22296960506226</v>
+      </c>
+      <c r="I29" s="1">
+        <v>117.22296960506226</v>
+      </c>
+      <c r="J29" s="1">
+        <v>142.65571961873661</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2.8154315052882642E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="1">
+        <v>4</v>
+      </c>
+      <c r="H30" s="1">
+        <v>3.2868775235470062</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.82171938088675156</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
+        <v>120.50984712860927</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.41252605422772426</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.47341237707532796</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.87138840090377345</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.4327198509645056</v>
+      </c>
+      <c r="K34" s="1">
+        <v>-0.90187742284312211</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1.7269295312985706</v>
+      </c>
+      <c r="M34" s="1">
+        <v>-0.90187742284312211</v>
+      </c>
+      <c r="N34" s="1">
+        <v>1.7269295312985706</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.75213387514724639</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6.2972444851643314E-2</v>
+      </c>
+      <c r="I35" s="2">
+        <v>11.943856982513502</v>
+      </c>
+      <c r="J35" s="2">
+        <v>2.8154315052882696E-4</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0.57729433887656334</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0.92697341141792944</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0.57729433887656334</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0.92697341141792944</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sorption isotherm results rewritten
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="64">
   <si>
     <t>Sorption Isotherm Comparison</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Sodium Montmorillonite</t>
+  </si>
+  <si>
+    <t>Tamamura</t>
   </si>
 </sst>
 </file>
@@ -323,7 +326,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -457,11 +459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256494544"/>
-        <c:axId val="256493760"/>
+        <c:axId val="474914288"/>
+        <c:axId val="474920952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="256494544"/>
+        <c:axId val="474914288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,12 +520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256493760"/>
+        <c:crossAx val="474920952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256493760"/>
+        <c:axId val="474920952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,7 +582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256494544"/>
+        <c:crossAx val="474914288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1483,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,6 +1880,112 @@
       </c>
       <c r="F19" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <f>0.03/100</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>6740.15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:B23" si="2">0.03/100</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>17749.39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>21473.27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>22894.86</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24">
+        <f>0.1/30</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>5.25</v>
+      </c>
+      <c r="E24">
+        <f>1/(0.03/30*0.1/0.97)</f>
+        <v>9700</v>
+      </c>
+      <c r="F24" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draft appropriate figures and tables
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -29,9 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="64">
   <si>
-    <t>Sorption Isotherm Comparison</t>
-  </si>
-  <si>
     <t>Mineral</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>Tamamura</t>
+  </si>
+  <si>
+    <t>Sorption Isotherm Comparison (Table 1)</t>
   </si>
 </sst>
 </file>
@@ -459,11 +459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474914288"/>
-        <c:axId val="474920952"/>
+        <c:axId val="494068208"/>
+        <c:axId val="494069776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474914288"/>
+        <c:axId val="494068208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,12 +520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474920952"/>
+        <c:crossAx val="494069776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474920952"/>
+        <c:axId val="494069776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474914288"/>
+        <c:crossAx val="494068208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1487,14 +1487,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1502,39 +1500,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <f>0.03/100</f>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -1543,19 +1541,19 @@
         <v>229.89</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B10" si="0">0.03/100</f>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1564,19 +1562,19 @@
         <v>471.37</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -1585,19 +1583,19 @@
         <v>2486.88</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>9</v>
@@ -1606,40 +1604,40 @@
         <v>115932.7</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1648,19 +1646,19 @@
         <v>302.74</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1669,19 +1667,19 @@
         <v>573.62</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1690,19 +1688,19 @@
         <v>11697.99</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <f>1/40</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>8.25</v>
@@ -1711,19 +1709,19 @@
         <v>1535</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <f>1/40</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>8.25</v>
@@ -1732,19 +1730,19 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <f t="shared" ref="B13:B14" si="1">1/40</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>8.25</v>
@@ -1753,19 +1751,19 @@
         <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>8.25</v>
@@ -1774,19 +1772,19 @@
         <v>174</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <f>0.1/10</f>
         <v>0.01</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>7</v>
@@ -1795,19 +1793,19 @@
         <v>1440.0319999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <f>0.1/10</f>
         <v>0.01</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -1816,19 +1814,19 @@
         <v>50.6</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <f>5/10</f>
         <v>0.5</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1837,19 +1835,19 @@
         <v>0.752</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <f>5/10</f>
         <v>0.5</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>10.1</v>
@@ -1858,19 +1856,19 @@
         <v>544</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <f>1/20</f>
         <v>0.05</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>6.5</v>
@@ -1879,19 +1877,19 @@
         <v>3724</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20">
         <f>0.03/100</f>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1900,19 +1898,19 @@
         <v>6740.15</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21">
         <f t="shared" ref="B21:B23" si="2">0.03/100</f>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1921,19 +1919,19 @@
         <v>17749.39</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <f t="shared" si="2"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22">
         <v>7</v>
@@ -1942,19 +1940,19 @@
         <v>21473.27</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23">
         <f t="shared" si="2"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23">
         <v>9</v>
@@ -1963,19 +1961,19 @@
         <v>22894.86</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24">
         <f>0.1/30</f>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24">
         <v>5.25</v>
@@ -1985,7 +1983,7 @@
         <v>9700</v>
       </c>
       <c r="F24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2010,19 +2008,19 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2057,7 +2055,7 @@
         <v>3594.28182437032</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -2077,7 +2075,7 @@
         <v>3051.5916575192095</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>0.99999926963558483</v>
@@ -2085,7 +2083,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1">
         <v>0.99999853927170312</v>
@@ -2094,7 +2092,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D6" s="6"/>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1">
         <v>0.99999707854340625</v>
@@ -2102,7 +2100,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1">
         <v>4.8406511408979136E-12</v>
@@ -2110,7 +2108,7 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2">
         <v>3</v>
@@ -2118,30 +2116,30 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -2161,7 +2159,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -2177,7 +2175,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
@@ -2193,33 +2191,33 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="1">
         <v>-1.549705240455168E-11</v>
@@ -2248,7 +2246,7 @@
     </row>
     <row r="18" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18" s="2">
         <v>3724.1309368597631</v>
@@ -2298,16 +2296,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2318,13 +2316,13 @@
         <v>880.67380000000003</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2335,7 +2333,7 @@
         <v>4701.3890000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2346,10 +2344,10 @@
         <v>9340.4390000000003</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -2361,10 +2359,10 @@
         <v>233.41942</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>0.99372706491098139</v>
@@ -2378,10 +2376,10 @@
         <v>899.29269999999997</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <v>0.98749347953659372</v>
@@ -2395,10 +2393,10 @@
         <v>1714.5220999999999</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <v>0.97498695907318744</v>
@@ -2412,10 +2410,10 @@
         <v>2479.904</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1">
         <v>670.02005546883538</v>
@@ -2429,10 +2427,10 @@
         <v>3192.3667</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
@@ -2440,30 +2438,30 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -2483,7 +2481,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -2499,7 +2497,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -2515,33 +2513,33 @@
     <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="1">
         <v>203.1510841687932</v>
@@ -2570,7 +2568,7 @@
     </row>
     <row r="19" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2">
         <v>1440.0320465648442</v>
@@ -2599,22 +2597,22 @@
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="1">
         <v>0.98756025859679031</v>
@@ -2622,7 +2620,7 @@
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1">
         <v>0.97527526435975931</v>
@@ -2630,7 +2628,7 @@
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1">
         <v>0.96703368581301241</v>
@@ -2638,7 +2636,7 @@
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="1">
         <v>215.3596181097262</v>
@@ -2646,7 +2644,7 @@
     </row>
     <row r="28" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2">
         <v>5</v>
@@ -2654,30 +2652,30 @@
     </row>
     <row r="30" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -2697,7 +2695,7 @@
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E33" s="1">
         <v>3</v>
@@ -2713,7 +2711,7 @@
     </row>
     <row r="34" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2729,33 +2727,33 @@
     <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="I36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="J36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="L36" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" s="1">
         <v>-48.596631511334635</v>
@@ -2784,7 +2782,7 @@
     </row>
     <row r="38" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38" s="2">
         <v>50.601522337114382</v>
@@ -2833,19 +2831,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3073,22 +3071,22 @@
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="1">
         <v>0.98626833922986679</v>
@@ -3096,7 +3094,7 @@
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1">
         <v>0.97272523696723956</v>
@@ -3104,7 +3102,7 @@
     </row>
     <row r="23" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" s="1">
         <v>0.96590654620904948</v>
@@ -3112,7 +3110,7 @@
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" s="1">
         <v>0.90648738595015843</v>
@@ -3120,7 +3118,7 @@
     </row>
     <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G25" s="2">
         <v>6</v>
@@ -3128,30 +3126,30 @@
     </row>
     <row r="27" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="29" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -3171,7 +3169,7 @@
     </row>
     <row r="30" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G30" s="1">
         <v>4</v>
@@ -3187,7 +3185,7 @@
     </row>
     <row r="31" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G31" s="2">
         <v>5</v>
@@ -3203,33 +3201,33 @@
     <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G34" s="1">
         <v>0.41252605422772426</v>
@@ -3258,7 +3256,7 @@
     </row>
     <row r="35" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G35" s="2">
         <v>0.75213387514724639</v>

</xml_diff>

<commit_message>
Changes to the draft, wording, focus... Moving toward more complex models of sorption
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -459,11 +459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="494068208"/>
-        <c:axId val="494069776"/>
+        <c:axId val="476241704"/>
+        <c:axId val="476242488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494068208"/>
+        <c:axId val="476241704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,12 +520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494069776"/>
+        <c:crossAx val="476242488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494069776"/>
+        <c:axId val="476242488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494068208"/>
+        <c:crossAx val="476241704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1487,7 +1487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated mineral properties with SA, calculated SA normalized Kd
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="66">
   <si>
     <t>Mineral</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Sorption Isotherm Comparison (Table 1)</t>
+  </si>
+  <si>
+    <t>K normalized by SA</t>
+  </si>
+  <si>
+    <t>SA</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -294,6 +300,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,11 +468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="476241704"/>
-        <c:axId val="476242488"/>
+        <c:axId val="191772792"/>
+        <c:axId val="184620992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="476241704"/>
+        <c:axId val="191772792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,12 +529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476242488"/>
+        <c:crossAx val="184620992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="476242488"/>
+        <c:axId val="184620992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476241704"/>
+        <c:crossAx val="191772792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1485,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:D25"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,12 +1509,12 @@
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1524,8 +1533,14 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1545,8 +1560,15 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="7">
+        <v>382.9</v>
+      </c>
+      <c r="H3">
+        <f>E3/G3</f>
+        <v>0.60039174719247845</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1566,8 +1588,15 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="7">
+        <v>382.9</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" ref="H4:H23" si="1">E4/G4</f>
+        <v>1.2310524941237921</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1587,8 +1616,15 @@
       <c r="F5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="7">
+        <v>382.9</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" si="1"/>
+        <v>6.4948550535387835</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1608,8 +1644,15 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="7">
+        <v>382.9</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="1"/>
+        <v>302.77539827631239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1629,8 +1672,10 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1650,8 +1695,15 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="8">
+        <v>146.46</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0670490236241976</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1671,8 +1723,15 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="8">
+        <v>146.46</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="1"/>
+        <v>3.9165642496244706</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1692,8 +1751,15 @@
       <c r="F10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="8">
+        <v>146.46</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="1"/>
+        <v>79.87156902908643</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1713,8 +1779,10 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="7"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1734,13 +1802,14 @@
       <c r="F12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:B14" si="1">1/40</f>
+        <f t="shared" ref="B13:B14" si="2">1/40</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C13" t="s">
@@ -1755,13 +1824,14 @@
       <c r="F13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C14" t="s">
@@ -1776,8 +1846,9 @@
       <c r="F14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1797,8 +1868,10 @@
       <c r="F15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="7"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1818,8 +1891,9 @@
       <c r="F16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1839,8 +1913,9 @@
       <c r="F17" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1860,8 +1935,9 @@
       <c r="F18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1881,8 +1957,9 @@
       <c r="F19" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1902,13 +1979,20 @@
       <c r="F20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="9">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H20" s="9">
+        <f t="shared" si="1"/>
+        <v>134.36764881783023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:B23" si="2">0.03/100</f>
+        <f t="shared" ref="B21:B23" si="3">0.03/100</f>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C21" t="s">
@@ -1923,13 +2007,20 @@
       <c r="F21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="9">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" si="1"/>
+        <v>353.8413540129979</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C22" t="s">
@@ -1944,13 +2035,20 @@
       <c r="F22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="9">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H22" s="9">
+        <f t="shared" si="1"/>
+        <v>428.07842590008374</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
       <c r="B23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C23" t="s">
@@ -1965,8 +2063,15 @@
       <c r="F23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="9">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="1"/>
+        <v>456.41840436984171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Filling in SAs from other studies
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
   <si>
     <t>Mineral</t>
   </si>
@@ -224,7 +224,10 @@
     <t>K normalized by SA</t>
   </si>
   <si>
-    <t>SA</t>
+    <t>SA (m2/g)</t>
+  </si>
+  <si>
+    <t>None reported</t>
   </si>
 </sst>
 </file>
@@ -468,11 +471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191772792"/>
-        <c:axId val="184620992"/>
+        <c:axId val="215437264"/>
+        <c:axId val="215441184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191772792"/>
+        <c:axId val="215437264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,12 +532,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184620992"/>
+        <c:crossAx val="215441184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184620992"/>
+        <c:axId val="215441184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,7 +594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191772792"/>
+        <c:crossAx val="215437264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1509,7 @@
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1672,7 +1675,9 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="9">
+        <v>146.46</v>
+      </c>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1779,8 +1784,13 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="7">
+        <v>253</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="1"/>
+        <v>6.0671936758893281</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1802,7 +1812,13 @@
       <c r="F12" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="G12">
+        <v>29</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="1"/>
+        <v>0.68965517241379315</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1824,7 +1840,13 @@
       <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="G13">
+        <v>24</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1846,6 +1868,9 @@
       <c r="F14" t="s">
         <v>14</v>
       </c>
+      <c r="G14">
+        <v>78</v>
+      </c>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,7 +1893,9 @@
       <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7">
+        <v>245</v>
+      </c>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1891,6 +1918,9 @@
       <c r="F16" t="s">
         <v>42</v>
       </c>
+      <c r="G16">
+        <v>23.6</v>
+      </c>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1934,6 +1964,9 @@
       </c>
       <c r="F18" t="s">
         <v>51</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
       </c>
       <c r="H18" s="9"/>
     </row>

</xml_diff>

<commit_message>
Pyrite SCM, Finished Applying Draft Changes, Some extra tables
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="70">
   <si>
     <t>Mineral</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Kd (mL/g)</t>
   </si>
   <si>
-    <t>Solid/Solution Ratio (g/mL)</t>
-  </si>
-  <si>
     <t>Seawater</t>
   </si>
   <si>
@@ -221,13 +218,25 @@
     <t>Sorption Isotherm Comparison (Table 1)</t>
   </si>
   <si>
-    <t>K normalized by SA</t>
-  </si>
-  <si>
     <t>SA (m2/g)</t>
   </si>
   <si>
     <t>None reported</t>
+  </si>
+  <si>
+    <t>Solid/Solution Ratio (mg/L)</t>
+  </si>
+  <si>
+    <t>K normalized by SA (mL/m2)</t>
+  </si>
+  <si>
+    <t>Pyrite</t>
+  </si>
+  <si>
+    <t>Clays society</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -471,11 +480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215437264"/>
-        <c:axId val="215441184"/>
+        <c:axId val="192795136"/>
+        <c:axId val="192802584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215437264"/>
+        <c:axId val="192795136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,12 +541,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215441184"/>
+        <c:crossAx val="192802584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215441184"/>
+        <c:axId val="192802584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215437264"/>
+        <c:crossAx val="192795136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1497,24 +1506,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1522,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1537,10 +1546,10 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1548,8 +1557,8 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <f>0.03/100</f>
-        <v>2.9999999999999997E-4</v>
+        <f t="shared" ref="B3:B10" si="0">30/0.1</f>
+        <v>300</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1575,9 +1584,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B10" si="0">0.03/100</f>
-        <v>2.9999999999999997E-4</v>
+      <c r="B4" s="9">
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1595,7 +1604,7 @@
         <v>382.9</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" ref="H4:H23" si="1">E4/G4</f>
+        <f t="shared" ref="H4:H28" si="1">E4/G4</f>
         <v>1.2310524941237921</v>
       </c>
     </row>
@@ -1603,9 +1612,9 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <v>300</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1631,9 +1640,9 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <v>300</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1659,9 +1668,9 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <v>300</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1684,9 +1693,9 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1712,9 +1721,9 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1740,9 +1749,9 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <v>300</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1769,11 +1778,11 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <f>1/40</f>
-        <v>2.5000000000000001E-2</v>
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>8.25</v>
@@ -1782,7 +1791,7 @@
         <v>1535</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="7">
         <v>253</v>
@@ -1796,12 +1805,12 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <f>1/40</f>
-        <v>2.5000000000000001E-2</v>
+      <c r="B12" s="9">
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>8.25</v>
@@ -1810,7 +1819,7 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>29</v>
@@ -1822,14 +1831,14 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13">
-        <f t="shared" ref="B13:B14" si="2">1/40</f>
-        <v>2.5000000000000001E-2</v>
+        <v>46</v>
+      </c>
+      <c r="B13" s="9">
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <v>8.25</v>
@@ -1838,7 +1847,7 @@
         <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <v>24</v>
@@ -1850,14 +1859,14 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
+        <v>47</v>
+      </c>
+      <c r="B14" s="9">
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>8.25</v>
@@ -1866,20 +1875,23 @@
         <v>174</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14">
         <v>78</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9">
+        <f t="shared" si="1"/>
+        <v>2.2307692307692308</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
-        <f>0.1/10</f>
-        <v>0.01</v>
+        <f>0.1/10*10^6</f>
+        <v>10000</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1891,20 +1903,23 @@
         <v>1440.0319999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="7">
         <v>245</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9">
+        <f t="shared" si="1"/>
+        <v>5.8776816326530605</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16">
-        <f>0.1/10</f>
-        <v>0.01</v>
+      <c r="B16" s="9">
+        <f>0.1/10*10^6</f>
+        <v>10000</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1916,23 +1931,26 @@
         <v>50.6</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16">
         <v>23.6</v>
       </c>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="9">
+        <f t="shared" si="1"/>
+        <v>2.1440677966101696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17">
-        <f>5/10</f>
-        <v>0.5</v>
+        <f>5/10*10^6</f>
+        <v>500000</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1941,20 +1959,25 @@
         <v>0.752</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18">
-        <f>5/10</f>
-        <v>0.5</v>
+        <f>5/10*10^6</f>
+        <v>500000</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18">
         <v>10.1</v>
@@ -1963,20 +1986,22 @@
         <v>544</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19">
-        <f>1/20</f>
-        <v>0.05</v>
+        <f>1/20*10^6</f>
+        <v>50000</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1988,17 +2013,26 @@
         <v>3724</v>
       </c>
       <c r="F19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19">
+        <v>97.42</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" si="1"/>
+        <v>38.226236912338329</v>
+      </c>
+      <c r="I19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20">
-        <f>0.03/100</f>
-        <v>2.9999999999999997E-4</v>
+      <c r="B20" s="9">
+        <f>30/0.1</f>
+        <v>300</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -2020,13 +2054,13 @@
         <v>134.36764881783023</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21">
-        <f t="shared" ref="B21:B23" si="3">0.03/100</f>
-        <v>2.9999999999999997E-4</v>
+        <v>60</v>
+      </c>
+      <c r="B21" s="9">
+        <f>30/0.1</f>
+        <v>300</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -2048,13 +2082,13 @@
         <v>353.8413540129979</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="3"/>
-        <v>2.9999999999999997E-4</v>
+        <v>60</v>
+      </c>
+      <c r="B22" s="9">
+        <f>30/0.1</f>
+        <v>300</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -2076,13 +2110,13 @@
         <v>428.07842590008374</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="3"/>
-        <v>2.9999999999999997E-4</v>
+        <v>60</v>
+      </c>
+      <c r="B23" s="9">
+        <f>30/0.1</f>
+        <v>300</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -2104,13 +2138,13 @@
         <v>456.41840436984171</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24">
-        <f>0.1/30</f>
-        <v>3.3333333333333335E-3</v>
+        <f>0.1/30*10^6</f>
+        <v>3333.3333333333335</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -2123,7 +2157,133 @@
         <v>9700</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="G24">
+        <v>31.82</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" si="1"/>
+        <v>304.83972344437461</v>
+      </c>
+      <c r="I24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="9">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="9">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="9">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="9">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="9">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>536</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="9">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="1"/>
+        <v>7824.8175182481746</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="9">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>520</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="9">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="1"/>
+        <v>7591.2408759124082</v>
       </c>
     </row>
   </sheetData>
@@ -2141,26 +2301,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2195,7 +2355,7 @@
         <v>3594.28182437032</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -2215,7 +2375,7 @@
         <v>3051.5916575192095</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1">
         <v>0.99999926963558483</v>
@@ -2223,7 +2383,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1">
         <v>0.99999853927170312</v>
@@ -2232,7 +2392,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D6" s="6"/>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1">
         <v>0.99999707854340625</v>
@@ -2240,7 +2400,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1">
         <v>4.8406511408979136E-12</v>
@@ -2248,7 +2408,7 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2">
         <v>3</v>
@@ -2256,30 +2416,30 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -2299,7 +2459,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -2315,7 +2475,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
@@ -2331,33 +2491,33 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="1">
         <v>-1.549705240455168E-11</v>
@@ -2386,7 +2546,7 @@
     </row>
     <row r="18" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" s="2">
         <v>3724.1309368597631</v>
@@ -2428,18 +2588,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -2456,13 +2616,13 @@
         <v>880.67380000000003</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2473,7 +2633,7 @@
         <v>4701.3890000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2484,10 +2644,10 @@
         <v>9340.4390000000003</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -2499,10 +2659,10 @@
         <v>233.41942</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1">
         <v>0.99372706491098139</v>
@@ -2516,10 +2676,10 @@
         <v>899.29269999999997</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1">
         <v>0.98749347953659372</v>
@@ -2533,10 +2693,10 @@
         <v>1714.5220999999999</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
         <v>0.97498695907318744</v>
@@ -2550,10 +2710,10 @@
         <v>2479.904</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1">
         <v>670.02005546883538</v>
@@ -2567,10 +2727,10 @@
         <v>3192.3667</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
@@ -2578,30 +2738,30 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -2621,7 +2781,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -2637,7 +2797,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -2653,33 +2813,33 @@
     <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1">
         <v>203.1510841687932</v>
@@ -2708,7 +2868,7 @@
     </row>
     <row r="19" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2">
         <v>1440.0320465648442</v>
@@ -2737,22 +2897,22 @@
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E24" s="1">
         <v>0.98756025859679031</v>
@@ -2760,7 +2920,7 @@
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="1">
         <v>0.97527526435975931</v>
@@ -2768,7 +2928,7 @@
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="1">
         <v>0.96703368581301241</v>
@@ -2776,7 +2936,7 @@
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" s="1">
         <v>215.3596181097262</v>
@@ -2784,7 +2944,7 @@
     </row>
     <row r="28" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2">
         <v>5</v>
@@ -2792,30 +2952,30 @@
     </row>
     <row r="30" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -2835,7 +2995,7 @@
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E33" s="1">
         <v>3</v>
@@ -2851,7 +3011,7 @@
     </row>
     <row r="34" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2867,33 +3027,33 @@
     <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="I36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="J36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="L36" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E37" s="1">
         <v>-48.596631511334635</v>
@@ -2922,7 +3082,7 @@
     </row>
     <row r="38" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38" s="2">
         <v>50.601522337114382</v>
@@ -2964,20 +3124,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3211,22 +3371,22 @@
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="1">
         <v>0.98626833922986679</v>
@@ -3234,7 +3394,7 @@
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" s="1">
         <v>0.97272523696723956</v>
@@ -3242,7 +3402,7 @@
     </row>
     <row r="23" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="1">
         <v>0.96590654620904948</v>
@@ -3250,7 +3410,7 @@
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" s="1">
         <v>0.90648738595015843</v>
@@ -3258,7 +3418,7 @@
     </row>
     <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" s="2">
         <v>6</v>
@@ -3266,30 +3426,30 @@
     </row>
     <row r="27" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -3309,7 +3469,7 @@
     </row>
     <row r="30" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G30" s="1">
         <v>4</v>
@@ -3325,7 +3485,7 @@
     </row>
     <row r="31" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G31" s="2">
         <v>5</v>
@@ -3341,33 +3501,33 @@
     <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G34" s="1">
         <v>0.41252605422772426</v>
@@ -3396,7 +3556,7 @@
     </row>
     <row r="35" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G35" s="2">
         <v>0.75213387514724639</v>

</xml_diff>

<commit_message>
Quick plots of the figures, edits to draft to reflect new figures, and small changes
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -17,6 +17,9 @@
     <sheet name="Sajih Data" sheetId="2" r:id="rId3"/>
     <sheet name="Nirdosh Data" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Compilation!$A$2:$I$2</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="69">
   <si>
     <t>Mineral</t>
   </si>
@@ -234,16 +237,13 @@
   </si>
   <si>
     <t>Clays society</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +253,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -300,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -315,6 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,11 +489,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="192795136"/>
-        <c:axId val="192802584"/>
+        <c:axId val="203079000"/>
+        <c:axId val="203082136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="192795136"/>
+        <c:axId val="203079000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,12 +550,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192802584"/>
+        <c:crossAx val="203082136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192802584"/>
+        <c:axId val="203082136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192795136"/>
+        <c:crossAx val="203079000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1509,7 +1518,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A24" sqref="A24:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,286 +1561,285 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B10" si="0">30/0.1</f>
+      <c r="B3" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <v>229.89</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="10">
         <v>382.9</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="10">
         <f>E3/G3</f>
         <v>0.60039174719247845</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
-        <f t="shared" si="0"/>
+      <c r="B4" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="10">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="10">
         <v>471.37</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="10">
         <v>382.9</v>
       </c>
-      <c r="H4" s="9">
-        <f t="shared" ref="H4:H28" si="1">E4/G4</f>
+      <c r="H4" s="10">
+        <f>E4/G4</f>
         <v>1.2310524941237921</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9">
-        <f t="shared" si="0"/>
+      <c r="B5" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="10">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10">
         <v>2486.88</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="10">
         <v>382.9</v>
       </c>
-      <c r="H5" s="9">
-        <f t="shared" si="1"/>
+      <c r="H5" s="10">
+        <f>E5/G5</f>
         <v>6.4948550535387835</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9">
-        <f t="shared" si="0"/>
+      <c r="B6" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="10">
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="10">
         <v>115932.7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="10">
         <v>382.9</v>
       </c>
-      <c r="H6" s="9">
-        <f t="shared" si="1"/>
+      <c r="H6" s="10">
+        <f>E6/G6</f>
         <v>302.77539827631239</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="9">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
+        <v>8.25</v>
+      </c>
+      <c r="E7">
+        <v>1535</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G7" s="9">
-        <v>146.46</v>
-      </c>
-      <c r="H7" s="9"/>
+        <v>253</v>
+      </c>
+      <c r="H7" s="9">
+        <f>E7/G7</f>
+        <v>6.0671936758893281</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9">
+        <f>0.1/10*10^6</f>
+        <v>10000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1440.0319999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="8">
+        <v>245</v>
+      </c>
+      <c r="H8" s="9">
+        <f>E8/G8</f>
+        <v>5.8776816326530605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9">
-        <f t="shared" si="0"/>
+      <c r="B9" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="10">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="10">
+        <v>146.46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10">
+        <f>30/0.1</f>
+        <v>300</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="10">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="E10" s="10">
         <v>302.74</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G10" s="10">
         <v>146.46</v>
       </c>
-      <c r="H8" s="9">
-        <f t="shared" si="1"/>
+      <c r="H10" s="10">
+        <f>E10/G10</f>
         <v>2.0670490236241976</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9">
-        <f t="shared" si="0"/>
+      <c r="B11" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D11" s="10">
         <v>7</v>
       </c>
-      <c r="E9">
+      <c r="E11" s="10">
         <v>573.62</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G11" s="10">
         <v>146.46</v>
       </c>
-      <c r="H9" s="9">
-        <f t="shared" si="1"/>
+      <c r="H11" s="10">
+        <f>E11/G11</f>
         <v>3.9165642496244706</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
-        <f t="shared" si="0"/>
+      <c r="B12" s="10">
+        <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D10">
+      <c r="D12" s="10">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="E12" s="10">
         <v>11697.99</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G12" s="10">
         <v>146.46</v>
       </c>
-      <c r="H10" s="9">
-        <f t="shared" si="1"/>
+      <c r="H12" s="10">
+        <f>E12/G12</f>
         <v>79.87156902908643</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <f>1/40*10^6</f>
-        <v>25000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>8.25</v>
-      </c>
-      <c r="E11">
-        <v>1535</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="7">
-        <v>253</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="1"/>
-        <v>6.0671936758893281</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="9">
-        <f>1/40*10^6</f>
-        <v>25000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>8.25</v>
-      </c>
-      <c r="E12">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12">
-        <v>29</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="1"/>
-        <v>0.68965517241379315</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B13" s="9">
         <f>1/40*10^6</f>
@@ -1844,270 +1852,259 @@
         <v>8.25</v>
       </c>
       <c r="E13">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="1"/>
-        <v>3.125</v>
+        <f>E13/G13</f>
+        <v>0.68965517241379315</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B14" s="9">
-        <f>1/40*10^6</f>
-        <v>25000</v>
+        <f>0.1/10*10^6</f>
+        <v>10000</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>8.25</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>174</v>
+        <v>50.6</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G14">
-        <v>78</v>
+        <v>23.6</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="1"/>
-        <v>2.2307692307692308</v>
+        <f>E14/G14</f>
+        <v>2.1440677966101696</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <f>0.1/10*10^6</f>
-        <v>10000</v>
+        <f>5/10*10^6</f>
+        <v>500000</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1440.0319999999999</v>
+        <v>0.752</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="7">
-        <v>245</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="shared" si="1"/>
-        <v>5.8776816326530605</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="9">
-        <f>0.1/10*10^6</f>
-        <v>10000</v>
+        <f>5/10*10^6</f>
+        <v>500000</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>10.1</v>
       </c>
       <c r="E16">
-        <v>50.6</v>
+        <v>544</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16">
-        <v>23.6</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="shared" si="1"/>
-        <v>2.1440677966101696</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B17">
-        <f>5/10*10^6</f>
-        <v>500000</v>
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>8.25</v>
       </c>
       <c r="E17">
-        <v>0.752</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>69</v>
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>24</v>
+      </c>
+      <c r="H17" s="9">
+        <f>E17/G17</f>
+        <v>3.125</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B18">
-        <f>5/10*10^6</f>
-        <v>500000</v>
+        <f>1/40*10^6</f>
+        <v>25000</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D18">
-        <v>10.1</v>
+        <v>8.25</v>
       </c>
       <c r="E18">
-        <v>544</v>
+        <v>174</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19">
-        <f>1/20*10^6</f>
-        <v>50000</v>
-      </c>
-      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>78</v>
+      </c>
+      <c r="H18" s="9">
+        <f>E18/G18</f>
+        <v>2.2307692307692308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="10">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D19">
-        <v>6.5</v>
-      </c>
-      <c r="E19">
-        <v>3724</v>
-      </c>
-      <c r="F19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19">
-        <v>97.42</v>
-      </c>
-      <c r="H19" s="9">
-        <f t="shared" si="1"/>
-        <v>38.226236912338329</v>
-      </c>
-      <c r="I19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="9">
-        <f>30/0.1</f>
-        <v>300</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D19" s="10">
+        <v>3</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="10">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="10">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>6740.15</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D20" s="10">
+        <v>5</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="9">
-        <v>50.161999999999999</v>
-      </c>
-      <c r="H20" s="9">
-        <f t="shared" si="1"/>
-        <v>134.36764881783023</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="9">
-        <f>30/0.1</f>
-        <v>300</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="G20" s="10">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="10">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-      <c r="E21">
-        <v>17749.39</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D21" s="10">
         <v>7</v>
       </c>
-      <c r="G21" s="9">
-        <v>50.161999999999999</v>
-      </c>
-      <c r="H21" s="9">
-        <f t="shared" si="1"/>
-        <v>353.8413540129979</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="9">
-        <f>30/0.1</f>
-        <v>300</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E21" s="10">
+        <v>536</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="10">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="H21" s="10">
+        <f>E21/G21</f>
+        <v>7824.8175182481746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="10">
+        <f>40/0.1</f>
+        <v>400</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="10">
+        <v>9</v>
+      </c>
+      <c r="E22" s="10">
+        <v>520</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E22">
-        <v>21473.27</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="9">
-        <v>50.161999999999999</v>
-      </c>
-      <c r="H22" s="9">
-        <f t="shared" si="1"/>
-        <v>428.07842590008374</v>
+      <c r="G22" s="10">
+        <f>AVERAGE(0.059,0.078)</f>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="H22" s="10">
+        <f>E22/G22</f>
+        <v>7591.2408759124082</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2115,178 +2112,182 @@
         <v>60</v>
       </c>
       <c r="B23" s="9">
+        <f>1/20*10^6</f>
+        <v>50000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>6.5</v>
+      </c>
+      <c r="E23">
+        <v>3724</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="9">
+        <v>97.42</v>
+      </c>
+      <c r="H23" s="9">
+        <f>E23/G23</f>
+        <v>38.226236912338329</v>
+      </c>
+      <c r="I23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="10">
         <f>30/0.1</f>
         <v>300</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D23">
+      <c r="D24" s="10">
+        <v>3</v>
+      </c>
+      <c r="E24" s="10">
+        <v>6740.15</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="10">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H24" s="10">
+        <f>E24/G24</f>
+        <v>134.36764881783023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="10">
+        <f>30/0.1</f>
+        <v>300</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="10">
+        <v>5</v>
+      </c>
+      <c r="E25" s="10">
+        <v>17749.39</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="10">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H25" s="10">
+        <f>E25/G25</f>
+        <v>353.8413540129979</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="10">
+        <f>30/0.1</f>
+        <v>300</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="10">
+        <v>7</v>
+      </c>
+      <c r="E26" s="10">
+        <v>21473.27</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="10">
+        <v>50.161999999999999</v>
+      </c>
+      <c r="H26" s="10">
+        <f>E26/G26</f>
+        <v>428.07842590008374</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="10">
+        <f>30/0.1</f>
+        <v>300</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="10">
         <v>9</v>
       </c>
-      <c r="E23">
+      <c r="E27" s="10">
         <v>22894.86</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G27" s="10">
         <v>50.161999999999999</v>
       </c>
-      <c r="H23" s="9">
-        <f t="shared" si="1"/>
+      <c r="H27" s="10">
+        <f>E27/G27</f>
         <v>456.41840436984171</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B24">
+      <c r="B28" s="9">
         <f>0.1/30*10^6</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D24">
+      <c r="D28">
         <v>5.25</v>
       </c>
-      <c r="E24">
+      <c r="E28">
         <f>1/(0.03/30*0.1/0.97)</f>
         <v>9700</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F28" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G24">
+      <c r="G28" s="9">
         <v>31.82</v>
       </c>
-      <c r="H24" s="9">
-        <f t="shared" si="1"/>
+      <c r="H28" s="9">
+        <f>E28/G28</f>
         <v>304.83972344437461</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="9">
-        <f>40/0.1</f>
-        <v>400</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="9">
-        <f>AVERAGE(0.059,0.078)</f>
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="H25" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="9">
-        <f>40/0.1</f>
-        <v>400</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="9">
-        <f>AVERAGE(0.059,0.078)</f>
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="H26" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="9">
-        <f>40/0.1</f>
-        <v>400</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="E27">
-        <v>536</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="9">
-        <f>AVERAGE(0.059,0.078)</f>
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="H27" s="9">
-        <f t="shared" si="1"/>
-        <v>7824.8175182481746</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="9">
-        <f>40/0.1</f>
-        <v>400</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>9</v>
-      </c>
-      <c r="E28">
-        <v>520</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="9">
-        <f>AVERAGE(0.059,0.078)</f>
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="H28" s="9">
-        <f t="shared" si="1"/>
-        <v>7591.2408759124082</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A2:I2">
+    <sortState ref="A3:I28">
+      <sortCondition ref="A2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Minor draft edits, figures should be complete
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SorptionKdComparison.xlsx
+++ b/Manuscript/Tables/SorptionKdComparison.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Manuscript\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\machen\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Manuscript\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11837"/>
   </bookViews>
   <sheets>
     <sheet name="Compilation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Compilation!$A$2:$I$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -480,6 +480,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4A4-4184-9FBB-AA45F4B68839}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1234,7 +1239,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1328,6 +1339,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1363,6 +1391,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1518,24 +1563,27 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD27"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="6" max="6" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1609,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1585,11 +1633,11 @@
         <v>382.9</v>
       </c>
       <c r="H3" s="10">
-        <f>E3/G3</f>
+        <f t="shared" ref="H3:H8" si="0">E3/G3</f>
         <v>0.60039174719247845</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -1613,11 +1661,11 @@
         <v>382.9</v>
       </c>
       <c r="H4" s="10">
-        <f>E4/G4</f>
+        <f t="shared" si="0"/>
         <v>1.2310524941237921</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
@@ -1641,11 +1689,11 @@
         <v>382.9</v>
       </c>
       <c r="H5" s="10">
-        <f>E5/G5</f>
+        <f t="shared" si="0"/>
         <v>6.4948550535387835</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
@@ -1669,11 +1717,11 @@
         <v>382.9</v>
       </c>
       <c r="H6" s="10">
-        <f>E6/G6</f>
+        <f t="shared" si="0"/>
         <v>302.77539827631239</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1697,11 +1745,11 @@
         <v>253</v>
       </c>
       <c r="H7" s="9">
-        <f>E7/G7</f>
+        <f t="shared" si="0"/>
         <v>6.0671936758893281</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1725,11 +1773,11 @@
         <v>245</v>
       </c>
       <c r="H8" s="9">
-        <f>E8/G8</f>
+        <f t="shared" si="0"/>
         <v>5.8776816326530605</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -1753,7 +1801,7 @@
         <v>146.46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
@@ -1781,7 +1829,7 @@
         <v>2.0670490236241976</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -1809,7 +1857,7 @@
         <v>3.9165642496244706</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -1837,7 +1885,7 @@
         <v>79.87156902908643</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1865,7 +1913,7 @@
         <v>0.68965517241379315</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1893,7 +1941,7 @@
         <v>2.1440677966101696</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1918,7 +1966,7 @@
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1943,7 +1991,7 @@
       </c>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1971,7 +2019,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1999,7 +2047,7 @@
         <v>2.2307692307692308</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
         <v>67</v>
       </c>
@@ -2024,7 +2072,7 @@
         <v>6.8500000000000005E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>67</v>
       </c>
@@ -2049,7 +2097,7 @@
         <v>6.8500000000000005E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>67</v>
       </c>
@@ -2074,11 +2122,11 @@
         <v>6.8500000000000005E-2</v>
       </c>
       <c r="H21" s="10">
-        <f>E21/G21</f>
+        <f t="shared" ref="H21:H28" si="1">E21/G21</f>
         <v>7824.8175182481746</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>67</v>
       </c>
@@ -2103,11 +2151,11 @@
         <v>6.8500000000000005E-2</v>
       </c>
       <c r="H22" s="10">
-        <f>E22/G22</f>
+        <f t="shared" si="1"/>
         <v>7591.2408759124082</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -2131,14 +2179,14 @@
         <v>97.42</v>
       </c>
       <c r="H23" s="9">
-        <f>E23/G23</f>
+        <f t="shared" si="1"/>
         <v>38.226236912338329</v>
       </c>
       <c r="I23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>60</v>
       </c>
@@ -2162,11 +2210,11 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H24" s="10">
-        <f>E24/G24</f>
+        <f t="shared" si="1"/>
         <v>134.36764881783023</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>60</v>
       </c>
@@ -2190,11 +2238,11 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H25" s="10">
-        <f>E25/G25</f>
+        <f t="shared" si="1"/>
         <v>353.8413540129979</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
         <v>60</v>
       </c>
@@ -2218,11 +2266,11 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H26" s="10">
-        <f>E26/G26</f>
+        <f t="shared" si="1"/>
         <v>428.07842590008374</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>60</v>
       </c>
@@ -2246,11 +2294,11 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H27" s="10">
-        <f>E27/G27</f>
+        <f t="shared" si="1"/>
         <v>456.41840436984171</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
         <v>60</v>
       </c>
@@ -2275,7 +2323,7 @@
         <v>31.82</v>
       </c>
       <c r="H28" s="9">
-        <f>E28/G28</f>
+        <f t="shared" si="1"/>
         <v>304.83972344437461</v>
       </c>
       <c r="I28" t="s">
@@ -2300,14 +2348,14 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2324,7 +2372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1.395E-9</v>
       </c>
@@ -2340,7 +2388,7 @@
         <v>3713.2616487455198</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>1.469E-10</v>
       </c>
@@ -2360,7 +2408,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="5">
         <v>1.822E-11</v>
       </c>
@@ -2382,7 +2430,7 @@
         <v>0.99999926963558483</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2390,7 +2438,7 @@
         <v>0.99999853927170312</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="D6" s="6"/>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -2399,7 +2447,7 @@
         <v>0.99999707854340625</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2407,7 +2455,7 @@
         <v>4.8406511408979136E-12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2415,12 +2463,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>28</v>
@@ -2438,7 +2486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2458,7 +2506,7 @@
         <v>7.6942262009724945E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="F13" s="1" t="s">
         <v>25</v>
       </c>
@@ -2474,7 +2522,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F14" s="2" t="s">
         <v>26</v>
       </c>
@@ -2488,8 +2536,8 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>33</v>
@@ -2516,7 +2564,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:14" x14ac:dyDescent="0.4">
       <c r="F17" s="1" t="s">
         <v>27</v>
       </c>
@@ -2545,7 +2593,7 @@
         <v>3.0823182259555064E-11</v>
       </c>
     </row>
-    <row r="18" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F18" s="2" t="s">
         <v>40</v>
       </c>
@@ -2587,15 +2635,15 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.61328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2609,7 +2657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0.71273874999999998</v>
       </c>
@@ -2626,7 +2674,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2.7491457000000001</v>
       </c>
@@ -2637,7 +2685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>6.4775114</v>
       </c>
@@ -2652,7 +2700,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>7.4571753000000003</v>
       </c>
@@ -2669,7 +2717,7 @@
         <v>0.99372706491098139</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>20.685638000000001</v>
       </c>
@@ -2686,7 +2734,7 @@
         <v>0.98749347953659372</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>32.391185999999998</v>
       </c>
@@ -2703,7 +2751,7 @@
         <v>0.97498695907318744</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>44.803916999999998</v>
       </c>
@@ -2720,7 +2768,7 @@
         <v>670.02005546883538</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>67.828575000000001</v>
       </c>
@@ -2737,12 +2785,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
         <v>28</v>
@@ -2760,7 +2808,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2780,7 +2828,7 @@
         <v>7.1344057367496438E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
@@ -2796,7 +2844,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
@@ -2810,8 +2858,8 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
         <v>33</v>
@@ -2838,7 +2886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2867,7 +2915,7 @@
         <v>8611.6313851240957</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
@@ -2896,7 +2944,7 @@
         <v>3499.1875104865571</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D21" t="s">
         <v>16</v>
       </c>
@@ -2904,14 +2952,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2919,7 +2967,7 @@
         <v>0.98756025859679031</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2927,7 +2975,7 @@
         <v>0.97527526435975931</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
@@ -2935,7 +2983,7 @@
         <v>0.96703368581301241</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D27" s="1" t="s">
         <v>21</v>
       </c>
@@ -2943,7 +2991,7 @@
         <v>215.3596181097262</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
@@ -2951,12 +2999,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
         <v>28</v>
@@ -2974,7 +3022,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D32" s="1" t="s">
         <v>24</v>
       </c>
@@ -2994,7 +3042,7 @@
         <v>1.6624127011823481E-3</v>
       </c>
     </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D33" s="1" t="s">
         <v>25</v>
       </c>
@@ -3010,7 +3058,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D34" s="2" t="s">
         <v>26</v>
       </c>
@@ -3024,8 +3072,8 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
         <v>33</v>
@@ -3052,7 +3100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.4">
       <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
@@ -3081,7 +3129,7 @@
         <v>548.73404619015332</v>
       </c>
     </row>
-    <row r="38" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D38" s="2" t="s">
         <v>40</v>
       </c>
@@ -3123,14 +3171,14 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -3147,7 +3195,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0.2</v>
       </c>
@@ -3166,7 +3214,7 @@
         <v>64.666666666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>0.4</v>
       </c>
@@ -3185,7 +3233,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>0.8</v>
       </c>
@@ -3204,7 +3252,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2.73</v>
       </c>
@@ -3223,7 +3271,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>3.64</v>
       </c>
@@ -3242,7 +3290,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>4.55</v>
       </c>
@@ -3261,7 +3309,7 @@
         <v>209.62790697674419</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>22.74</v>
       </c>
@@ -3280,7 +3328,7 @@
         <v>3787.9999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>0.33537894000000001</v>
       </c>
@@ -3295,7 +3343,7 @@
         <v>0.51256575621593881</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>0.64073210000000003</v>
       </c>
@@ -3310,7 +3358,7 @@
         <v>0.79853868722981103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B11">
         <v>1.2517366000000001</v>
       </c>
@@ -3325,7 +3373,7 @@
         <v>0.85098462408145614</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>1.6840321</v>
       </c>
@@ -3340,7 +3388,7 @@
         <v>1.1968493355916434</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13">
         <v>7.5865210000000003</v>
       </c>
@@ -3355,7 +3403,7 @@
         <v>1.0042100984100617</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>16.631900000000002</v>
       </c>
@@ -3370,7 +3418,7 @@
         <v>0.73654561415111908</v>
       </c>
     </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F18" t="s">
         <v>16</v>
       </c>
@@ -3378,14 +3426,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3393,7 +3441,7 @@
         <v>0.98626833922986679</v>
       </c>
     </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3401,7 +3449,7 @@
         <v>0.97272523696723956</v>
       </c>
     </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3409,7 +3457,7 @@
         <v>0.96590654620904948</v>
       </c>
     </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3417,7 +3465,7 @@
         <v>0.90648738595015843</v>
       </c>
     </row>
-    <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F25" s="2" t="s">
         <v>22</v>
       </c>
@@ -3425,12 +3473,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
         <v>28</v>
@@ -3448,7 +3496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F29" s="1" t="s">
         <v>24</v>
       </c>
@@ -3468,7 +3516,7 @@
         <v>2.8154315052882642E-4</v>
       </c>
     </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:11" x14ac:dyDescent="0.4">
       <c r="F30" s="1" t="s">
         <v>25</v>
       </c>
@@ -3484,7 +3532,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F31" s="2" t="s">
         <v>26</v>
       </c>
@@ -3498,8 +3546,8 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.4">
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
         <v>33</v>
@@ -3526,7 +3574,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.4">
       <c r="F34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3555,7 +3603,7 @@
         <v>1.7269295312985706</v>
       </c>
     </row>
-    <row r="35" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F35" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>